<commit_message>
adicionado referencia na tabela
Agora cada tabela possui sua identificaçãopara facilitar seu desenvolvimento
</commit_message>
<xml_diff>
--- a/BANCO_DE_DADOS/modelo-V4.xlsx
+++ b/BANCO_DE_DADOS/modelo-V4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Cheshire\BANCO_DE_DADOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEEC363-A2BA-4E04-9FCB-8584DD737620}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C9D77B-66F6-4641-88C8-11721B543694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BBE51270-7034-41B5-9215-58623F8F8CCD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="118">
   <si>
     <t>login_fk</t>
   </si>
@@ -257,57 +257,6 @@
     <t>estado</t>
   </si>
   <si>
-    <t>PESSOA</t>
-  </si>
-  <si>
-    <t>MENSAGEM</t>
-  </si>
-  <si>
-    <t>TELEFONE</t>
-  </si>
-  <si>
-    <t>LOGIN</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>ENDERECO</t>
-  </si>
-  <si>
-    <t>REGISTRO</t>
-  </si>
-  <si>
-    <t>TIPO_USUARIO</t>
-  </si>
-  <si>
-    <t>IDENTIFICACAO_ALUNO</t>
-  </si>
-  <si>
-    <t>DADOS_FAMILIARES</t>
-  </si>
-  <si>
-    <t>DADOS_MAE</t>
-  </si>
-  <si>
-    <t>DADOS_PAI</t>
-  </si>
-  <si>
-    <t>DADOS_RESPONSAVEL</t>
-  </si>
-  <si>
-    <t>HISTORICO_SAUDE</t>
-  </si>
-  <si>
-    <t>ANAMNESE</t>
-  </si>
-  <si>
-    <t>DESENVOLVIMENTO</t>
-  </si>
-  <si>
-    <t>ESCOLARIZACAO</t>
-  </si>
-  <si>
     <t>id_endereco</t>
   </si>
   <si>
@@ -387,6 +336,57 @@
   </si>
   <si>
     <t>necessita_apoio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MENSAGEM - 1.0 </t>
+  </si>
+  <si>
+    <t>PESSOA - 2.0</t>
+  </si>
+  <si>
+    <t>TELEFONE - 2.1</t>
+  </si>
+  <si>
+    <t>EMAIL - 2.2</t>
+  </si>
+  <si>
+    <t>LOGIN - 2.3</t>
+  </si>
+  <si>
+    <t>ENDERECO - 2.4</t>
+  </si>
+  <si>
+    <t>REGISTRO - 2.5</t>
+  </si>
+  <si>
+    <t>TIPO_USUARIO - 2.6</t>
+  </si>
+  <si>
+    <t>ANAMNESE - 3.0</t>
+  </si>
+  <si>
+    <t>IDENTIFICACAO_ALUNO - 3.1</t>
+  </si>
+  <si>
+    <t>DADOS_FAMILIARES - 3.2</t>
+  </si>
+  <si>
+    <t>HISTORICO_SAUDE - 3.3</t>
+  </si>
+  <si>
+    <t>DESENVOLVIMENTO - 3.4</t>
+  </si>
+  <si>
+    <t>ESCOLARIZACAO - 3.5</t>
+  </si>
+  <si>
+    <t>DADOS_MAE - 3.2.1</t>
+  </si>
+  <si>
+    <t>DADOS_PAI - 3.2.2</t>
+  </si>
+  <si>
+    <t>DADOS_RESPONSAVEL - 3.2.3</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -538,7 +538,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -546,7 +545,57 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -858,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157789B8-057F-4D33-BC28-7CE04553AB3A}">
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,39 +917,39 @@
     <col min="2" max="2" width="3.28515625" style="9" customWidth="1"/>
     <col min="3" max="3" width="15" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="1.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.7109375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2" style="9" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="1.7109375" style="9" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2" style="9" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="1.7109375" style="8" customWidth="1"/>
-    <col min="15" max="15" width="22.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="1.7109375" style="9" customWidth="1"/>
     <col min="17" max="17" width="32.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="1.7109375" style="9" customWidth="1"/>
     <col min="19" max="19" width="23.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="1.7109375" style="9" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="4" style="9" customWidth="1"/>
-    <col min="23" max="23" width="30.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="3" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="I1" s="10"/>
       <c r="O1" s="1" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="W1" s="9"/>
     </row>
@@ -912,7 +961,7 @@
       <c r="C2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="19"/>
+      <c r="E2" s="18"/>
       <c r="O2" s="15" t="s">
         <v>27</v>
       </c>
@@ -929,6 +978,7 @@
       <c r="O3" s="13" t="s">
         <v>35</v>
       </c>
+      <c r="U3" s="18"/>
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -992,53 +1042,53 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B9" s="8"/>
       <c r="W9" s="9"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="2" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="W10" s="5" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="15" t="s">
@@ -1051,7 +1101,7 @@
         <v>4</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="K11" s="15" t="s">
         <v>12</v>
@@ -1068,16 +1118,16 @@
       <c r="S11" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="U11" s="17" t="s">
-        <v>108</v>
+      <c r="U11" s="16" t="s">
+        <v>91</v>
       </c>
       <c r="W11" s="16" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="13" t="s">
@@ -1108,10 +1158,10 @@
         <v>69</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="W12" t="s">
-        <v>110</v>
+        <v>85</v>
+      </c>
+      <c r="W12" s="4" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -1141,10 +1191,10 @@
         <v>71</v>
       </c>
       <c r="U13" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="W13" t="s">
-        <v>112</v>
+        <v>86</v>
+      </c>
+      <c r="W13" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1165,13 +1215,13 @@
         <v>46</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="U14" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="W14" t="s">
-        <v>111</v>
+        <v>87</v>
+      </c>
+      <c r="W14" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -1192,13 +1242,13 @@
         <v>42</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="U15" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="W15" t="s">
-        <v>113</v>
+        <v>88</v>
+      </c>
+      <c r="W15" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -1213,13 +1263,13 @@
         <v>43</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="U16" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="W16" t="s">
-        <v>114</v>
+        <v>89</v>
+      </c>
+      <c r="W16" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -1231,13 +1281,13 @@
         <v>58</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="U17" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="W17" t="s">
-        <v>115</v>
+        <v>90</v>
+      </c>
+      <c r="W17" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
@@ -1246,22 +1296,22 @@
         <v>39</v>
       </c>
       <c r="S18" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="W18" t="s">
-        <v>116</v>
+        <v>79</v>
+      </c>
+      <c r="W18" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
       <c r="Q19" s="7" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="S19" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="W19" t="s">
-        <v>117</v>
+        <v>80</v>
+      </c>
+      <c r="W19" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
@@ -1270,6 +1320,7 @@
       <c r="Q20" s="15" t="s">
         <v>47</v>
       </c>
+      <c r="W20" s="9"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
@@ -1289,18 +1340,21 @@
       <c r="Q21" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="W21" s="9"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O22" s="10"/>
       <c r="Q22" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="W22" s="9"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O23" s="10"/>
       <c r="Q23" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="W23" s="9"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I24" s="10"/>
@@ -1308,98 +1362,123 @@
       <c r="Q24" s="3" t="s">
         <v>67</v>
       </c>
+      <c r="W24" s="9"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O25" s="10"/>
       <c r="Q25" s="13" t="s">
         <v>51</v>
       </c>
+      <c r="W25" s="9"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O26" s="10"/>
       <c r="Q26" s="13" t="s">
         <v>56</v>
       </c>
+      <c r="W26" s="9"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W27" s="9"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="Q28" s="7" t="s">
-        <v>85</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="W28" s="9"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="Q29" s="15" t="s">
         <v>52</v>
       </c>
+      <c r="W29" s="9"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="Q30" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="W30" s="9"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="Q31" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="W31" s="9"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="Q32" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="W32" s="9"/>
     </row>
     <row r="33" spans="15:23" x14ac:dyDescent="0.25">
       <c r="Q33" s="3" t="s">
         <v>66</v>
       </c>
+      <c r="W33" s="9"/>
     </row>
     <row r="34" spans="15:23" x14ac:dyDescent="0.25">
       <c r="Q34" s="13" t="s">
         <v>55</v>
       </c>
+      <c r="W34" s="9"/>
     </row>
     <row r="35" spans="15:23" x14ac:dyDescent="0.25">
       <c r="Q35" s="13" t="s">
         <v>57</v>
       </c>
+      <c r="W35" s="9"/>
+    </row>
+    <row r="36" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="W36" s="9"/>
     </row>
     <row r="37" spans="15:23" x14ac:dyDescent="0.25">
       <c r="Q37" s="7" t="s">
-        <v>86</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="W37" s="9"/>
     </row>
     <row r="38" spans="15:23" x14ac:dyDescent="0.25">
       <c r="Q38" s="15" t="s">
         <v>59</v>
       </c>
+      <c r="W38" s="9"/>
     </row>
     <row r="39" spans="15:23" x14ac:dyDescent="0.25">
       <c r="Q39" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="W39" s="9"/>
     </row>
     <row r="40" spans="15:23" x14ac:dyDescent="0.25">
       <c r="Q40" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="W40" s="9"/>
     </row>
     <row r="41" spans="15:23" x14ac:dyDescent="0.25">
       <c r="Q41" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="W41" s="9"/>
     </row>
     <row r="42" spans="15:23" x14ac:dyDescent="0.25">
       <c r="Q42" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="W42" s="9"/>
     </row>
     <row r="43" spans="15:23" x14ac:dyDescent="0.25">
       <c r="Q43" s="13" t="s">
         <v>64</v>
       </c>
+      <c r="W43" s="9"/>
     </row>
     <row r="44" spans="15:23" x14ac:dyDescent="0.25">
       <c r="Q44" s="13" t="s">
         <v>65</v>
       </c>
+      <c r="W44" s="9"/>
     </row>
     <row r="45" spans="15:23" x14ac:dyDescent="0.25">
       <c r="O45" s="8"/>
@@ -1413,12 +1492,35 @@
       <c r="W45" s="8"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:W1048576">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="id_">
+      <formula>NOT(ISERROR(SEARCH("id_",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="_fk">
+      <formula>NOT(ISERROR(SEARCH("_fk",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010093FD3C0481E2AB4C8FA676162B890140" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61293849ff2bc0008f677c11e4bd9e18">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9be52ef7-c563-4948-a796-0f95658e087f" xmlns:ns4="4128e3ff-bd25-4b7e-822e-228ddd53df9a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9162a302901a7085921fc43a47315066" ns3:_="" ns4:_="">
     <xsd:import namespace="9be52ef7-c563-4948-a796-0f95658e087f"/>
@@ -1627,22 +1729,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E96F33E6-2A48-4FE3-9B40-FF90F34C074D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CF6D65F-EA34-4141-84D4-DAD80346F99A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{785794D2-5A6F-4B80-B483-16449ABF54CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1659,21 +1763,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CF6D65F-EA34-4141-84D4-DAD80346F99A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E96F33E6-2A48-4FE3-9B40-FF90F34C074D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
correcção planilha + completando script
correção ortográfica na planilha
+
completando o script que irá formar o banco de dados - a construção básica das tabelas foi feita, falta criar as referencias
</commit_message>
<xml_diff>
--- a/BANCO_DE_DADOS/modelo-V4.xlsx
+++ b/BANCO_DE_DADOS/modelo-V4.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Cheshire\BANCO_DE_DADOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C9D77B-66F6-4641-88C8-11721B543694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BBE51270-7034-41B5-9215-58623F8F8CCD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="bd_cheshire_V4" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -242,9 +241,6 @@
     <t>historico_saude_fk</t>
   </si>
   <si>
-    <t>cuidados medicos</t>
-  </si>
-  <si>
     <t>id_historico_saude</t>
   </si>
   <si>
@@ -387,12 +383,15 @@
   </si>
   <si>
     <t>DADOS_RESPONSAVEL - 3.2.3</t>
+  </si>
+  <si>
+    <t>cuidados_medicos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -545,7 +544,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -557,41 +556,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -904,11 +868,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157789B8-057F-4D33-BC28-7CE04553AB3A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" topLeftCell="V4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF34" sqref="AF34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,15 +905,15 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I1" s="10"/>
       <c r="O1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="W1" s="9"/>
     </row>
@@ -1042,53 +1006,53 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="8"/>
       <c r="W9" s="9"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="I10" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="K10" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="M10" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="O10" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q10" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="Q10" s="5" t="s">
+      <c r="S10" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="S10" s="5" t="s">
+      <c r="U10" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="U10" s="5" t="s">
+      <c r="W10" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="W10" s="5" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="15" t="s">
@@ -1101,7 +1065,7 @@
         <v>4</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K11" s="15" t="s">
         <v>12</v>
@@ -1116,25 +1080,25 @@
         <v>41</v>
       </c>
       <c r="S11" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U11" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="W11" s="16" t="s">
         <v>91</v>
-      </c>
-      <c r="W11" s="16" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>3</v>
@@ -1155,13 +1119,13 @@
         <v>44</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -1188,13 +1152,13 @@
         <v>45</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U13" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1215,13 +1179,13 @@
         <v>46</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="U14" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -1242,19 +1206,19 @@
         <v>42</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U15" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B16" s="8"/>
       <c r="I16" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O16" s="6" t="s">
         <v>28</v>
@@ -1263,13 +1227,13 @@
         <v>43</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U16" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -1281,13 +1245,13 @@
         <v>58</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U17" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="W17" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
@@ -1296,22 +1260,22 @@
         <v>39</v>
       </c>
       <c r="S18" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W18" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
       <c r="Q19" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S19" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W19" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
@@ -1383,7 +1347,7 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="Q28" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W28" s="9"/>
     </row>
@@ -1434,7 +1398,7 @@
     </row>
     <row r="37" spans="15:23" x14ac:dyDescent="0.25">
       <c r="Q37" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W37" s="9"/>
     </row>
@@ -1512,15 +1476,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010093FD3C0481E2AB4C8FA676162B890140" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61293849ff2bc0008f677c11e4bd9e18">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9be52ef7-c563-4948-a796-0f95658e087f" xmlns:ns4="4128e3ff-bd25-4b7e-822e-228ddd53df9a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9162a302901a7085921fc43a47315066" ns3:_="" ns4:_="">
     <xsd:import namespace="9be52ef7-c563-4948-a796-0f95658e087f"/>
@@ -1729,6 +1684,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E96F33E6-2A48-4FE3-9B40-FF90F34C074D}">
   <ds:schemaRefs>
@@ -1739,14 +1703,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CF6D65F-EA34-4141-84D4-DAD80346F99A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{785794D2-5A6F-4B80-B483-16449ABF54CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1763,4 +1719,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CF6D65F-EA34-4141-84D4-DAD80346F99A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
identificação da tabela "identificacao_aluno"
Alterei de "rm" para "id_aluno", assim seguindo padrão de todas as outras tabelas
</commit_message>
<xml_diff>
--- a/BANCO_DE_DADOS/modelo-V4.xlsx
+++ b/BANCO_DE_DADOS/modelo-V4.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="119">
   <si>
     <t>login_fk</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t>cuidados_medicos</t>
+  </si>
+  <si>
+    <t>id_aluno</t>
   </si>
 </sst>
 </file>
@@ -871,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF34" sqref="AF34"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1077,7 @@
         <v>18</v>
       </c>
       <c r="O11" s="15" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="Q11" s="15" t="s">
         <v>41</v>
@@ -1476,6 +1479,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010093FD3C0481E2AB4C8FA676162B890140" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61293849ff2bc0008f677c11e4bd9e18">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9be52ef7-c563-4948-a796-0f95658e087f" xmlns:ns4="4128e3ff-bd25-4b7e-822e-228ddd53df9a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9162a302901a7085921fc43a47315066" ns3:_="" ns4:_="">
     <xsd:import namespace="9be52ef7-c563-4948-a796-0f95658e087f"/>
@@ -1684,15 +1696,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E96F33E6-2A48-4FE3-9B40-FF90F34C074D}">
   <ds:schemaRefs>
@@ -1703,6 +1706,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CF6D65F-EA34-4141-84D4-DAD80346F99A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{785794D2-5A6F-4B80-B483-16449ABF54CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1719,12 +1730,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CF6D65F-EA34-4141-84D4-DAD80346F99A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adicionado campo na tabela "endereco"
campo "numero" adicionado na planilha
</commit_message>
<xml_diff>
--- a/BANCO_DE_DADOS/modelo-V4.xlsx
+++ b/BANCO_DE_DADOS/modelo-V4.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="119">
   <si>
     <t>login_fk</t>
   </si>
@@ -551,14 +551,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -874,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,7 +1170,7 @@
         <v>8</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>17</v>
@@ -1197,7 +1197,7 @@
         <v>9</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>14</v>
@@ -1221,7 +1221,7 @@
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B16" s="8"/>
       <c r="I16" s="3" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="O16" s="6" t="s">
         <v>28</v>
@@ -1241,6 +1241,9 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
+      <c r="I17" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="O17" s="6" t="s">
         <v>29</v>
       </c>
@@ -1459,12 +1462,12 @@
       <c r="W45" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W1048576">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="id_">
+  <conditionalFormatting sqref="A18:W1048576 A1:W13 A14:H17 J14:W17 I15:I17">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="_fk">
+      <formula>NOT(ISERROR(SEARCH("_fk",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="id_">
       <formula>NOT(ISERROR(SEARCH("id_",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="_fk">
-      <formula>NOT(ISERROR(SEARCH("_fk",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1479,15 +1482,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010093FD3C0481E2AB4C8FA676162B890140" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61293849ff2bc0008f677c11e4bd9e18">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9be52ef7-c563-4948-a796-0f95658e087f" xmlns:ns4="4128e3ff-bd25-4b7e-822e-228ddd53df9a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9162a302901a7085921fc43a47315066" ns3:_="" ns4:_="">
     <xsd:import namespace="9be52ef7-c563-4948-a796-0f95658e087f"/>
@@ -1696,6 +1690,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E96F33E6-2A48-4FE3-9B40-FF90F34C074D}">
   <ds:schemaRefs>
@@ -1706,14 +1709,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CF6D65F-EA34-4141-84D4-DAD80346F99A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{785794D2-5A6F-4B80-B483-16449ABF54CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1730,4 +1725,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CF6D65F-EA34-4141-84D4-DAD80346F99A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
acrescentado campo "data-aenviada" em mensagem
O campo "enviada" e dentro da tabela "mensagem" para armazenar o momento em que a mensagem foi enviada para o usuario
</commit_message>
<xml_diff>
--- a/BANCO_DE_DADOS/modelo-V4.xlsx
+++ b/BANCO_DE_DADOS/modelo-V4.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Cheshire\BANCO_DE_DADOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0914825-BC39-4AB4-B1E2-3C2F24D77740}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bd_cheshire_V4" sheetId="1" r:id="rId1"/>
@@ -19,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="120">
   <si>
     <t>login_fk</t>
   </si>
@@ -389,12 +382,15 @@
   </si>
   <si>
     <t>id_aluno</t>
+  </si>
+  <si>
+    <t>data_enviada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -871,11 +867,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,7 +985,7 @@
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>119</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="14" t="s">
@@ -1002,21 +998,21 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="8"/>
       <c r="W8" s="9"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="B9" s="8"/>
       <c r="W9" s="9"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="2" t="s">
@@ -1055,7 +1051,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="15" t="s">
@@ -1094,7 +1090,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="13" t="s">
@@ -1132,6 +1128,9 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="B13" s="8"/>
       <c r="C13" s="3" t="s">
         <v>7</v>
@@ -1462,7 +1461,7 @@
       <c r="W45" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A18:W1048576 A1:W13 A14:H17 J14:W17 I15:I17">
+  <conditionalFormatting sqref="A18:W1048576 J14:W17 A1:W6 B7:W13 A15:I17 B14:H14 A8:A13">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="_fk">
       <formula>NOT(ISERROR(SEARCH("_fk",A1)))</formula>
     </cfRule>
@@ -1476,12 +1475,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010093FD3C0481E2AB4C8FA676162B890140" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61293849ff2bc0008f677c11e4bd9e18">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9be52ef7-c563-4948-a796-0f95658e087f" xmlns:ns4="4128e3ff-bd25-4b7e-822e-228ddd53df9a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9162a302901a7085921fc43a47315066" ns3:_="" ns4:_="">
     <xsd:import namespace="9be52ef7-c563-4948-a796-0f95658e087f"/>
@@ -1690,16 +1698,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CF6D65F-EA34-4141-84D4-DAD80346F99A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E96F33E6-2A48-4FE3-9B40-FF90F34C074D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1708,7 +1715,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{785794D2-5A6F-4B80-B483-16449ABF54CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1725,12 +1732,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CF6D65F-EA34-4141-84D4-DAD80346F99A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>